<commit_message>
Trimmed some data, updated GAMs, updated figures
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE132DF-884E-43F3-A120-ABB123BD5426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787C7121-F519-4891-9C45-C855E41DFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
   <si>
     <t>Species</t>
   </si>
@@ -159,15 +159,9 @@
     <t>thr.pheno</t>
   </si>
   <si>
-    <t>7.554; 8.818</t>
-  </si>
-  <si>
     <t>thr.geo</t>
   </si>
   <si>
-    <t>29; 29</t>
-  </si>
-  <si>
     <t>vc.pheno</t>
   </si>
   <si>
@@ -193,6 +187,42 @@
   </si>
   <si>
     <t>lv.temp.sal</t>
+  </si>
+  <si>
+    <t>lv.2d</t>
+  </si>
+  <si>
+    <t>8.3; 8.818</t>
+  </si>
+  <si>
+    <t>19.566; 27.731</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>eg.base</t>
+  </si>
+  <si>
+    <t>27.763; 27.091</t>
+  </si>
+  <si>
+    <t>8.447; 1.00</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>8.583; 6.902</t>
+  </si>
+  <si>
+    <t>27.930; 27.351</t>
+  </si>
+  <si>
+    <t>NRS</t>
+  </si>
+  <si>
+    <t>PC</t>
   </si>
 </sst>
 </file>
@@ -578,7 +608,8 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -587,7 +618,8 @@
     <col min="2" max="2" width="8.7265625" style="1"/>
     <col min="3" max="3" width="12.31640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.1328125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="10.76953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.2265625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.04296875" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.1328125" style="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
@@ -649,10 +681,10 @@
         <v>19</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>9</v>
@@ -681,16 +713,16 @@
         <v>0.70099999999999996</v>
       </c>
       <c r="F2" s="6">
-        <v>8101.9</v>
+        <v>7876.6</v>
       </c>
       <c r="G2" s="6">
-        <v>16160.83</v>
+        <v>15707.05</v>
       </c>
       <c r="H2" s="6">
-        <v>25.327000000000002</v>
+        <v>25.8</v>
       </c>
       <c r="I2" s="6">
-        <v>8.8030000000000008</v>
+        <v>8.7929999999999993</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -716,25 +748,25 @@
         <v>20</v>
       </c>
       <c r="E3" s="4">
-        <v>0.76100000000000001</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="F3" s="6">
-        <v>7651.7</v>
+        <v>7453.3</v>
       </c>
       <c r="G3" s="6">
-        <v>15219.88</v>
+        <v>14805.92</v>
       </c>
       <c r="H3" s="6">
-        <v>24.896999999999998</v>
+        <v>26.279</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="M3" s="6">
-        <v>2.1080000000000001</v>
+        <v>2.2850000000000001</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -753,23 +785,23 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="4">
         <v>0.73499999999999999</v>
       </c>
       <c r="F4" s="6">
-        <v>7892.8</v>
+        <v>7680.2</v>
       </c>
       <c r="G4" s="6">
-        <v>15686.81</v>
+        <v>15255.47</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6">
-        <v>9</v>
+        <v>8.6609999999999996</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K4" s="6">
         <v>2.2850000000000001</v>
@@ -793,22 +825,22 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4">
-        <v>0.75800000000000001</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="F5" s="6">
-        <v>7690.9</v>
+        <v>7477.2</v>
       </c>
       <c r="G5" s="6">
-        <v>15284.03</v>
+        <v>14852.47</v>
       </c>
       <c r="H5" s="6">
-        <v>25.670999999999999</v>
+        <v>26.068000000000001</v>
       </c>
       <c r="I5" s="6">
-        <v>7.5209999999999999</v>
+        <v>7.6680000000000001</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -816,7 +848,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6">
-        <v>9.1129999999999995</v>
+        <v>9.1219999999999999</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -833,19 +865,19 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4">
         <v>0.73</v>
       </c>
       <c r="F6" s="6">
-        <v>7970.5</v>
+        <v>7751.3</v>
       </c>
       <c r="G6" s="6">
-        <v>15774.73</v>
+        <v>15342.01</v>
       </c>
       <c r="H6" s="6">
-        <v>23.788</v>
+        <v>23.262</v>
       </c>
       <c r="I6" s="6">
         <v>8.7639999999999993</v>
@@ -855,7 +887,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6">
-        <v>26.361000000000001</v>
+        <v>26.155999999999999</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -863,17 +895,20 @@
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.75">
+      <c r="A7" s="5">
+        <v>44540</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4">
-        <v>0.64400000000000002</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F7" s="6">
         <v>6135.9</v>
@@ -898,14 +933,17 @@
       <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.75">
+      <c r="A8" s="5">
+        <v>44540</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>0.65500000000000003</v>
@@ -935,14 +973,17 @@
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.75">
+      <c r="A9" s="5">
+        <v>44540</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4">
         <v>0.68100000000000005</v>
@@ -972,14 +1013,17 @@
       <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.75">
+      <c r="A10" s="5">
+        <v>44540</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4">
         <v>0.69199999999999995</v>
@@ -1011,11 +1055,33 @@
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="E11" s="4"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="A11" s="5">
+        <v>44540</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5967</v>
+      </c>
+      <c r="G11" s="6">
+        <v>11841.88</v>
+      </c>
+      <c r="H11" s="6">
+        <v>24.721</v>
+      </c>
+      <c r="I11" s="6">
+        <v>5.9240000000000004</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1024,14 +1090,38 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+      <c r="R11" s="6">
+        <v>25.802</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="A12" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="F12" s="6">
+        <v>7266.1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>14493.3</v>
+      </c>
+      <c r="H12" s="6">
+        <v>27.952999999999999</v>
+      </c>
+      <c r="I12" s="6">
+        <v>8.2319999999999993</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1043,14 +1133,36 @@
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="E13" s="4"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="A13" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F13" s="6">
+        <v>7216.7</v>
+      </c>
+      <c r="G13" s="6">
+        <v>14384.02</v>
+      </c>
+      <c r="H13" s="6">
+        <v>27.594999999999999</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="L13" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -1059,12 +1171,34 @@
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="A14" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F14" s="6">
+        <v>7080.7</v>
+      </c>
+      <c r="G14" s="6">
+        <v>14029.54</v>
+      </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="I14" s="6">
+        <v>8.24</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -1075,43 +1209,113 @@
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="A15" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="F15" s="6">
+        <v>7245.5</v>
+      </c>
+      <c r="G15" s="6">
+        <v>14430.7</v>
+      </c>
+      <c r="H15" s="6">
+        <v>27.634</v>
+      </c>
+      <c r="I15" s="6">
+        <v>7.3609999999999998</v>
+      </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="O15" s="6">
+        <v>7.2779999999999996</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="A16" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.745</v>
+      </c>
+      <c r="F16" s="6">
+        <v>7141.1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>14079</v>
+      </c>
+      <c r="H16" s="6">
+        <v>27.234999999999999</v>
+      </c>
+      <c r="I16" s="6">
+        <v>7.9779999999999998</v>
+      </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
+      <c r="N16" s="6">
+        <v>28.013000000000002</v>
+      </c>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
     </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A17" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3773.6</v>
+      </c>
+      <c r="G17" s="6">
+        <v>7429.91</v>
+      </c>
+      <c r="H17" s="6">
+        <v>28.07</v>
+      </c>
+      <c r="I17" s="6">
+        <v>5.67</v>
+      </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -1122,28 +1326,74 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A18" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="F18" s="6">
+        <v>3768</v>
+      </c>
+      <c r="G18" s="6">
+        <v>7414.87</v>
+      </c>
+      <c r="H18" s="6">
+        <v>28.048999999999999</v>
+      </c>
+      <c r="I18" s="6">
+        <v>5.6559999999999997</v>
+      </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="P18" s="6">
+        <v>3.59</v>
+      </c>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E19" s="4"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A19" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="F19" s="6">
+        <v>3681.6</v>
+      </c>
+      <c r="G19" s="6">
+        <v>7222.5429999999997</v>
+      </c>
+      <c r="H19" s="6">
+        <v>28.073</v>
+      </c>
+      <c r="I19" s="6">
+        <v>5.38</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1151,31 +1401,81 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
+      <c r="Q19" s="6">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E20" s="4"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A20" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="F20" s="6">
+        <v>3672.6</v>
+      </c>
+      <c r="G20" s="6">
+        <v>7199.55</v>
+      </c>
+      <c r="H20" s="6">
+        <v>28.048999999999999</v>
+      </c>
+      <c r="I20" s="6">
+        <v>5.2859999999999996</v>
+      </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
+      <c r="P20" s="6">
+        <v>4.1420000000000003</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>8.4740000000000002</v>
+      </c>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E21" s="4"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A21" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="F21" s="6">
+        <v>3600.6</v>
+      </c>
+      <c r="G21" s="6">
+        <v>7026.5</v>
+      </c>
+      <c r="H21" s="6">
+        <v>27.751000000000001</v>
+      </c>
+      <c r="I21" s="6">
+        <v>5.5129999999999999</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1184,14 +1484,38 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="R21" s="6">
+        <v>25.245999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A22" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.504</v>
+      </c>
+      <c r="F22" s="6">
+        <v>15361</v>
+      </c>
+      <c r="G22" s="6">
+        <v>30823.279999999999</v>
+      </c>
+      <c r="H22" s="6">
+        <v>27.297000000000001</v>
+      </c>
+      <c r="I22" s="6">
+        <v>6.5579999999999998</v>
+      </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
@@ -1202,15 +1526,37 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A23" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="F23" s="6">
+        <v>15311</v>
+      </c>
+      <c r="G23" s="6">
+        <v>30684.85</v>
+      </c>
+      <c r="H23" s="6">
+        <v>27.361999999999998</v>
+      </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="L23" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -1218,13 +1564,35 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E24" s="4"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A24" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="F24" s="6">
+        <v>15110</v>
+      </c>
+      <c r="G24" s="6">
+        <v>30202.71</v>
+      </c>
       <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="I24" s="6">
+        <v>7.3559999999999999</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1234,44 +1602,114 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E25" s="4"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A25" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F25" s="6">
+        <v>15317</v>
+      </c>
+      <c r="G25" s="6">
+        <v>30688.91</v>
+      </c>
+      <c r="H25" s="6">
+        <v>27.478999999999999</v>
+      </c>
+      <c r="I25" s="6">
+        <v>7.5579999999999998</v>
+      </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
+      <c r="O25" s="6">
+        <v>8.1170000000000009</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E26" s="4"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A26" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="F26" s="6">
+        <v>15187</v>
+      </c>
+      <c r="G26" s="6">
+        <v>30279.1</v>
+      </c>
+      <c r="H26" s="6">
+        <v>27.379000000000001</v>
+      </c>
+      <c r="I26" s="6">
+        <v>7.1859999999999999</v>
+      </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
+      <c r="N26" s="6">
+        <v>28.228000000000002</v>
+      </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A27" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="F27" s="6">
+        <v>11069</v>
+      </c>
+      <c r="G27" s="6">
+        <v>22167.02</v>
+      </c>
+      <c r="H27" s="6">
+        <v>27.061</v>
+      </c>
+      <c r="I27" s="6">
+        <v>5.7320000000000002</v>
+      </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -1282,28 +1720,74 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E28" s="4"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A28" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="F28" s="6">
+        <v>11000</v>
+      </c>
+      <c r="G28" s="6">
+        <v>22006.69</v>
+      </c>
+      <c r="H28" s="6">
+        <v>26.87</v>
+      </c>
+      <c r="I28" s="6">
+        <v>5.758</v>
+      </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
+      <c r="P28" s="6">
+        <v>7.99</v>
+      </c>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E29" s="4"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A29" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="F29" s="6">
+        <v>10859</v>
+      </c>
+      <c r="G29" s="6">
+        <v>21700.16</v>
+      </c>
+      <c r="H29" s="6">
+        <v>27.701000000000001</v>
+      </c>
+      <c r="I29" s="6">
+        <v>5.6820000000000004</v>
+      </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
@@ -1311,31 +1795,81 @@
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
+      <c r="Q29" s="6">
+        <v>7.7389999999999999</v>
+      </c>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E30" s="4"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A30" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="F30" s="6">
+        <v>10842</v>
+      </c>
+      <c r="G30" s="6">
+        <v>21657.24</v>
+      </c>
+      <c r="H30" s="6">
+        <v>27.603999999999999</v>
+      </c>
+      <c r="I30" s="6">
+        <v>5.6859999999999999</v>
+      </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
+      <c r="P30" s="6">
+        <v>7.1870000000000003</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>7.6719999999999997</v>
+      </c>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E31" s="4"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A31" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="F31" s="6">
+        <v>10835</v>
+      </c>
+      <c r="G31" s="6">
+        <v>21635.51</v>
+      </c>
+      <c r="H31" s="6">
+        <v>27.58</v>
+      </c>
+      <c r="I31" s="6">
+        <v>5.6449999999999996</v>
+      </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
@@ -1344,14 +1878,38 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-    </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E32" s="4"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="R31" s="6">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A32" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="F32" s="6">
+        <v>6128.5</v>
+      </c>
+      <c r="G32" s="6">
+        <v>12221.21</v>
+      </c>
+      <c r="H32" s="6">
+        <v>26.602</v>
+      </c>
+      <c r="I32" s="6">
+        <v>7.9160000000000004</v>
+      </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
@@ -1362,28 +1920,74 @@
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
     </row>
-    <row r="33" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E33" s="4"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A33" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F33" s="6">
+        <v>6125.9</v>
+      </c>
+      <c r="G33" s="6">
+        <v>12211.7</v>
+      </c>
+      <c r="H33" s="6">
+        <v>26.626999999999999</v>
+      </c>
+      <c r="I33" s="6">
+        <v>5.81</v>
+      </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
+      <c r="P33" s="6">
+        <v>5.0380000000000003</v>
+      </c>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
     </row>
-    <row r="34" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E34" s="4"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A34" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0.68</v>
+      </c>
+      <c r="F34" s="6">
+        <v>6031.7</v>
+      </c>
+      <c r="G34" s="6">
+        <v>11994.29</v>
+      </c>
+      <c r="H34" s="6">
+        <v>26.86</v>
+      </c>
+      <c r="I34" s="6">
+        <v>5.5780000000000003</v>
+      </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
@@ -1391,31 +1995,81 @@
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
+      <c r="Q34" s="6">
+        <v>8.6519999999999992</v>
+      </c>
       <c r="R34" s="6"/>
     </row>
-    <row r="35" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E35" s="4"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A35" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="F35" s="6">
+        <v>6033.1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>11998.75</v>
+      </c>
+      <c r="H35" s="6">
+        <v>26.765000000000001</v>
+      </c>
+      <c r="I35" s="6">
+        <v>5.5519999999999996</v>
+      </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
+      <c r="P35" s="6">
+        <v>2.9239999999999999</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>8.657</v>
+      </c>
       <c r="R35" s="6"/>
     </row>
-    <row r="36" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E36" s="4"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A36" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="F36" s="6">
+        <v>5988.7</v>
+      </c>
+      <c r="G36" s="6">
+        <v>11876.23</v>
+      </c>
+      <c r="H36" s="6">
+        <v>26.213999999999999</v>
+      </c>
+      <c r="I36" s="6">
+        <v>5.5819999999999999</v>
+      </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
@@ -1424,14 +2078,38 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-    </row>
-    <row r="37" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E37" s="4"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="R36" s="6">
+        <v>25.085000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A37" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="F37" s="6">
+        <v>3839</v>
+      </c>
+      <c r="G37" s="6">
+        <v>7603.26</v>
+      </c>
+      <c r="H37" s="6">
+        <v>26.965</v>
+      </c>
+      <c r="I37" s="6">
+        <v>5.8869999999999996</v>
+      </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
@@ -1442,28 +2120,74 @@
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
     </row>
-    <row r="38" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E38" s="4"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A38" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="F38" s="6">
+        <v>3826.2</v>
+      </c>
+      <c r="G38" s="6">
+        <v>7574.18</v>
+      </c>
+      <c r="H38" s="6">
+        <v>26.824999999999999</v>
+      </c>
+      <c r="I38" s="6">
+        <v>5.0330000000000004</v>
+      </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
+      <c r="P38" s="6">
+        <v>5.6509999999999998</v>
+      </c>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
     </row>
-    <row r="39" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E39" s="4"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A39" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F39" s="6">
+        <v>3819.7</v>
+      </c>
+      <c r="G39" s="6">
+        <v>7553.2889999999998</v>
+      </c>
+      <c r="H39" s="6">
+        <v>27.007000000000001</v>
+      </c>
+      <c r="I39" s="6">
+        <v>5.343</v>
+      </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
@@ -1471,31 +2195,81 @@
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
+      <c r="Q39" s="6">
+        <v>6.5869999999999997</v>
+      </c>
       <c r="R39" s="6"/>
     </row>
-    <row r="40" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E40" s="4"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A40" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="F40" s="6">
+        <v>3801.9</v>
+      </c>
+      <c r="G40" s="6">
+        <v>7516.3310000000001</v>
+      </c>
+      <c r="H40" s="6">
+        <v>26.861000000000001</v>
+      </c>
+      <c r="I40" s="6">
+        <v>5.0839999999999996</v>
+      </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
+      <c r="P40" s="6">
+        <v>5.73</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>6.008</v>
+      </c>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="5:18" x14ac:dyDescent="0.75">
-      <c r="E41" s="4"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A41" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="F41" s="6">
+        <v>3754.3</v>
+      </c>
+      <c r="G41" s="6">
+        <v>7373.4189999999999</v>
+      </c>
+      <c r="H41" s="6">
+        <v>26.971</v>
+      </c>
+      <c r="I41" s="6">
+        <v>5.085</v>
+      </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
@@ -1504,9 +2278,14 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-    </row>
-    <row r="42" spans="5:18" x14ac:dyDescent="0.75">
+      <c r="R41" s="6">
+        <v>24.41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A42" s="5">
+        <v>44543</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
@@ -1522,7 +2301,10 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A43" s="5">
+        <v>44543</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
@@ -1538,7 +2320,10 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A44" s="5">
+        <v>44543</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
@@ -1554,7 +2339,10 @@
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A45" s="5">
+        <v>44543</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -1570,7 +2358,10 @@
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A46" s="5">
+        <v>44543</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -1586,7 +2377,10 @@
       <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A47" s="5">
+        <v>44543</v>
+      </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -1602,7 +2396,10 @@
       <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A48" s="5">
+        <v>44543</v>
+      </c>
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -1618,7 +2415,10 @@
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
     </row>
-    <row r="49" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="A49" s="5">
+        <v>44543</v>
+      </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -1634,7 +2434,7 @@
       <c r="Q49" s="6"/>
       <c r="R49" s="6"/>
     </row>
-    <row r="50" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -1650,7 +2450,7 @@
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E51" s="4"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -1666,7 +2466,7 @@
       <c r="Q51" s="6"/>
       <c r="R51" s="6"/>
     </row>
-    <row r="52" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E52" s="4"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -1682,7 +2482,7 @@
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E53" s="4"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -1698,7 +2498,7 @@
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
     </row>
-    <row r="54" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E54" s="4"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -1714,7 +2514,7 @@
       <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
     </row>
-    <row r="55" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E55" s="4"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -1730,7 +2530,7 @@
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
     </row>
-    <row r="56" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E56" s="4"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -1746,7 +2546,7 @@
       <c r="Q56" s="6"/>
       <c r="R56" s="6"/>
     </row>
-    <row r="57" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E57" s="4"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
@@ -1762,7 +2562,7 @@
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
     </row>
-    <row r="58" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E58" s="4"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -1778,7 +2578,7 @@
       <c r="Q58" s="6"/>
       <c r="R58" s="6"/>
     </row>
-    <row r="59" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E59" s="4"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
@@ -1794,7 +2594,7 @@
       <c r="Q59" s="6"/>
       <c r="R59" s="6"/>
     </row>
-    <row r="60" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E60" s="4"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -1810,7 +2610,7 @@
       <c r="Q60" s="6"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E61" s="4"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -1826,7 +2626,7 @@
       <c r="Q61" s="6"/>
       <c r="R61" s="6"/>
     </row>
-    <row r="62" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E62" s="4"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -1842,7 +2642,7 @@
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
     </row>
-    <row r="63" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E63" s="4"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -1858,7 +2658,7 @@
       <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="5:18" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E64" s="4"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>

</xml_diff>

<commit_message>
Trimming, redoing GAMs, checking outputs
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787C7121-F519-4891-9C45-C855E41DFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF1AE4F-1308-414E-ABB9-F13348D47226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
+    <workbookView xWindow="520" yWindow="430" windowWidth="15995" windowHeight="6420" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="47">
   <si>
     <t>Species</t>
   </si>
@@ -223,6 +223,18 @@
   </si>
   <si>
     <t>PC</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>YFS</t>
+  </si>
+  <si>
+    <t>3.99; 6.112</t>
+  </si>
+  <si>
+    <t>27.109; 26.940</t>
   </si>
 </sst>
 </file>
@@ -607,9 +619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0069B89D-77AC-4F26-B032-0EC1CFE3B568}">
   <dimension ref="A1:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1163,7 +1175,9 @@
       <c r="L13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="6"/>
+      <c r="M13" s="6">
+        <v>2.048</v>
+      </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -1199,7 +1213,9 @@
       <c r="J14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6">
+        <v>2.121</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -1557,7 +1573,9 @@
       <c r="L23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="6"/>
+      <c r="M23" s="6">
+        <v>1.0488</v>
+      </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -1593,7 +1611,9 @@
       <c r="J24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="6">
+        <v>1.0842000000000001</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
@@ -2286,11 +2306,30 @@
       <c r="A42" s="5">
         <v>44543</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="B42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="F42" s="6">
+        <v>4865.8999999999996</v>
+      </c>
+      <c r="G42" s="6">
+        <v>9651.8799999999992</v>
+      </c>
+      <c r="H42" s="6">
+        <v>27.808</v>
+      </c>
+      <c r="I42" s="6">
+        <v>5.5229999999999997</v>
+      </c>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
@@ -2305,15 +2344,36 @@
       <c r="A43" s="5">
         <v>44543</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="B43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F43" s="6">
+        <v>4817.5</v>
+      </c>
+      <c r="G43" s="6">
+        <v>9547.268</v>
+      </c>
+      <c r="H43" s="6">
+        <v>27.765000000000001</v>
+      </c>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
+      <c r="L43" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M43" s="6">
+        <v>2.0169999999999999</v>
+      </c>
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -2324,13 +2384,34 @@
       <c r="A44" s="5">
         <v>44543</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F44" s="6">
+        <v>4580.7</v>
+      </c>
+      <c r="G44" s="6">
+        <v>9004.2510000000002</v>
+      </c>
       <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
+      <c r="I44" s="6">
+        <v>7.8869999999999996</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K44" s="6">
+        <v>2.2850000000000001</v>
+      </c>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
@@ -2343,17 +2424,38 @@
       <c r="A45" s="5">
         <v>44543</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
+      <c r="B45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="F45" s="6">
+        <v>4847.5</v>
+      </c>
+      <c r="G45" s="6">
+        <v>9602.6669999999995</v>
+      </c>
+      <c r="H45" s="6">
+        <v>27.756</v>
+      </c>
+      <c r="I45" s="6">
+        <v>5.1840000000000002</v>
+      </c>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
+      <c r="O45" s="6">
+        <v>6.2750000000000004</v>
+      </c>
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
@@ -2362,16 +2464,37 @@
       <c r="A46" s="5">
         <v>44543</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
+      <c r="B46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="4">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="F46" s="6">
+        <v>4726.5</v>
+      </c>
+      <c r="G46" s="6">
+        <v>9317.1419999999998</v>
+      </c>
+      <c r="H46" s="6">
+        <v>20.838999999999999</v>
+      </c>
+      <c r="I46" s="6">
+        <v>8.0250000000000004</v>
+      </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
+      <c r="N46" s="6">
+        <v>21.994</v>
+      </c>
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
@@ -2381,11 +2504,30 @@
       <c r="A47" s="5">
         <v>44543</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="B47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="4">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F47" s="6">
+        <v>4002.2</v>
+      </c>
+      <c r="G47" s="6">
+        <v>7927.0129999999999</v>
+      </c>
+      <c r="H47" s="6">
+        <v>26.266999999999999</v>
+      </c>
+      <c r="I47" s="6">
+        <v>5.8179999999999996</v>
+      </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -2400,18 +2542,39 @@
       <c r="A48" s="5">
         <v>44543</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
+      <c r="B48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="F48" s="6">
+        <v>3982.8</v>
+      </c>
+      <c r="G48" s="6">
+        <v>7872.8720000000003</v>
+      </c>
+      <c r="H48" s="6">
+        <v>26.303999999999998</v>
+      </c>
+      <c r="I48" s="6">
+        <v>5.83</v>
+      </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
+      <c r="P48" s="6">
+        <v>7.016</v>
+      </c>
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
     </row>
@@ -2419,11 +2582,30 @@
       <c r="A49" s="5">
         <v>44543</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
+      <c r="B49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="F49" s="6">
+        <v>3848</v>
+      </c>
+      <c r="G49" s="6">
+        <v>7604.3320000000003</v>
+      </c>
+      <c r="H49" s="6">
+        <v>25.678999999999998</v>
+      </c>
+      <c r="I49" s="6">
+        <v>5.1749999999999998</v>
+      </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
@@ -2431,31 +2613,81 @@
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
+      <c r="Q49" s="6">
+        <v>8.423</v>
+      </c>
       <c r="R49" s="6"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.75">
-      <c r="E50" s="4"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
+      <c r="A50" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="F50" s="6">
+        <v>3827.2</v>
+      </c>
+      <c r="G50" s="6">
+        <v>7548.3649999999998</v>
+      </c>
+      <c r="H50" s="6">
+        <v>25.768999999999998</v>
+      </c>
+      <c r="I50" s="6">
+        <v>5.1959999999999997</v>
+      </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-      <c r="Q50" s="6"/>
+      <c r="P50" s="6">
+        <v>6.8079999999999998</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>8.4949999999999992</v>
+      </c>
       <c r="R50" s="6"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.75">
-      <c r="E51" s="4"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
+      <c r="A51" s="5">
+        <v>44543</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="F51" s="6">
+        <v>3751.9</v>
+      </c>
+      <c r="G51" s="6">
+        <v>7358.0079999999998</v>
+      </c>
+      <c r="H51" s="6">
+        <v>25.966000000000001</v>
+      </c>
+      <c r="I51" s="6">
+        <v>5.0709999999999997</v>
+      </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
@@ -2464,7 +2696,9 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
+      <c r="R51" s="6">
+        <v>25.713000000000001</v>
+      </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.75">
       <c r="E52" s="4"/>

</xml_diff>

<commit_message>
Creating better explanatory figures, checking models
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF1AE4F-1308-414E-ABB9-F13348D47226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C15D9A2-C7E8-456A-BDC2-5194D9F7B2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="430" windowWidth="15995" windowHeight="6420" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
+    <workbookView xWindow="8830" yWindow="25" windowWidth="10345" windowHeight="7745" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GAM Outputs" sheetId="1" r:id="rId1"/>
+    <sheet name="Temp-Sal Values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="59">
   <si>
     <t>Species</t>
   </si>
@@ -235,6 +236,42 @@
   </si>
   <si>
     <t>27.109; 26.940</t>
+  </si>
+  <si>
+    <t>Yellowfin Sole</t>
+  </si>
+  <si>
+    <t>Alaska Plaice</t>
+  </si>
+  <si>
+    <t>Flathead Sole</t>
+  </si>
+  <si>
+    <t>Northern Rock Sole</t>
+  </si>
+  <si>
+    <t>Pacific Cod</t>
+  </si>
+  <si>
+    <t>Walleye Pollock</t>
+  </si>
+  <si>
+    <t>Sal 1st Quartile</t>
+  </si>
+  <si>
+    <t>Sal Median</t>
+  </si>
+  <si>
+    <t>Sal 3rd Quartile</t>
+  </si>
+  <si>
+    <t>Temp 1st Quartile</t>
+  </si>
+  <si>
+    <t>Temp Median</t>
+  </si>
+  <si>
+    <t>Temp 3rd Quartile</t>
   </si>
 </sst>
 </file>
@@ -619,9 +656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0069B89D-77AC-4F26-B032-0EC1CFE3B568}">
   <dimension ref="A1:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2076,19 +2113,19 @@
         <v>31</v>
       </c>
       <c r="E36" s="4">
-        <v>0.69899999999999995</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="F36" s="6">
-        <v>5988.7</v>
+        <v>5944.3</v>
       </c>
       <c r="G36" s="6">
-        <v>11876.23</v>
+        <v>11791.08</v>
       </c>
       <c r="H36" s="6">
-        <v>26.213999999999999</v>
+        <v>26.198</v>
       </c>
       <c r="I36" s="6">
-        <v>5.5819999999999999</v>
+        <v>5.55</v>
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -2099,7 +2136,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6">
-        <v>25.085000000000001</v>
+        <v>24.907</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.75">
@@ -3703,4 +3740,186 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F6249F-90A6-4965-B716-979738F67B12}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="15.58984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.40625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>31.486000000000001</v>
+      </c>
+      <c r="C2">
+        <v>31.646999999999998</v>
+      </c>
+      <c r="D2">
+        <v>31.632000000000001</v>
+      </c>
+      <c r="E2">
+        <v>31.658999999999999</v>
+      </c>
+      <c r="F2">
+        <v>31.608000000000001</v>
+      </c>
+      <c r="G2">
+        <v>30.326000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>31.686</v>
+      </c>
+      <c r="C3">
+        <v>31.835000000000001</v>
+      </c>
+      <c r="D3">
+        <v>31.818000000000001</v>
+      </c>
+      <c r="E3">
+        <v>31.844000000000001</v>
+      </c>
+      <c r="F3">
+        <v>31.86</v>
+      </c>
+      <c r="G3">
+        <v>30.983000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>31.890999999999998</v>
+      </c>
+      <c r="C4">
+        <v>32.024999999999999</v>
+      </c>
+      <c r="D4">
+        <v>32.036000000000001</v>
+      </c>
+      <c r="E4">
+        <v>32.119</v>
+      </c>
+      <c r="F4">
+        <v>32.128</v>
+      </c>
+      <c r="G4">
+        <v>31.474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>4.2709999999999999</v>
+      </c>
+      <c r="C5">
+        <v>2.2309999999999999</v>
+      </c>
+      <c r="D5">
+        <v>2.3660000000000001</v>
+      </c>
+      <c r="E5">
+        <v>3.1850000000000001</v>
+      </c>
+      <c r="F5">
+        <v>2.758</v>
+      </c>
+      <c r="G5">
+        <v>8.8279999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>5.423</v>
+      </c>
+      <c r="C6">
+        <v>4.2539999999999996</v>
+      </c>
+      <c r="D6">
+        <v>4.3289999999999997</v>
+      </c>
+      <c r="E6">
+        <v>4.5549999999999997</v>
+      </c>
+      <c r="F6">
+        <v>4.4119999999999999</v>
+      </c>
+      <c r="G6">
+        <v>9.5939999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>6.0121000000000002</v>
+      </c>
+      <c r="C7">
+        <v>5.8319999999999999</v>
+      </c>
+      <c r="D7">
+        <v>5.5460000000000003</v>
+      </c>
+      <c r="E7">
+        <v>5.3949999999999996</v>
+      </c>
+      <c r="F7">
+        <v>5.7830000000000004</v>
+      </c>
+      <c r="G7">
+        <v>10.766</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on other thesis materials, improving some code
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96636E78-C7CF-4CEE-932B-95AF0357678F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE80853-9D9A-48F0-9B8C-5E272ED80132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8830" yWindow="25" windowWidth="10345" windowHeight="7745" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM Outputs" sheetId="1" r:id="rId1"/>
     <sheet name="Temp-Sal Values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -657,9 +656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0069B89D-77AC-4F26-B032-0EC1CFE3B568}">
   <dimension ref="A1:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R37" sqref="R37"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -946,7 +945,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A7" s="5">
-        <v>44540</v>
+        <v>44561</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -958,19 +957,19 @@
         <v>25</v>
       </c>
       <c r="E7" s="4">
-        <v>0.63700000000000001</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="F7" s="6">
-        <v>6135.9</v>
+        <v>5112.8999999999996</v>
       </c>
       <c r="G7" s="6">
-        <v>12243.74</v>
+        <v>10212.049999999999</v>
       </c>
       <c r="H7" s="6">
-        <v>26.364000000000001</v>
+        <v>26.177</v>
       </c>
       <c r="I7" s="6">
-        <v>5.9480000000000004</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -984,7 +983,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A8" s="5">
-        <v>44540</v>
+        <v>44561</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -996,19 +995,19 @@
         <v>26</v>
       </c>
       <c r="E8" s="4">
-        <v>0.65500000000000003</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="F8" s="6">
-        <v>6105.5</v>
+        <v>5084.2</v>
       </c>
       <c r="G8" s="6">
-        <v>12180.95</v>
+        <v>10151.33</v>
       </c>
       <c r="H8" s="6">
-        <v>25.215</v>
+        <v>25.106000000000002</v>
       </c>
       <c r="I8" s="6">
-        <v>5.9509999999999996</v>
+        <v>5.4320000000000004</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -1017,14 +1016,14 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6">
-        <v>6.3520000000000003</v>
+        <v>5.9859999999999998</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A9" s="5">
-        <v>44540</v>
+        <v>44561</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -1036,19 +1035,19 @@
         <v>29</v>
       </c>
       <c r="E9" s="4">
-        <v>0.68100000000000005</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="F9" s="6">
-        <v>6030.1</v>
+        <v>5090.3999999999996</v>
       </c>
       <c r="G9" s="6">
-        <v>12005.26</v>
+        <v>10158.700000000001</v>
       </c>
       <c r="H9" s="6">
-        <v>25.727</v>
+        <v>25.762</v>
       </c>
       <c r="I9" s="6">
-        <v>5.9320000000000004</v>
+        <v>4.71</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1058,13 +1057,13 @@
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6">
-        <v>8.5860000000000003</v>
+        <v>7.5709999999999997</v>
       </c>
       <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A10" s="5">
-        <v>44540</v>
+        <v>44561</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -1076,19 +1075,19 @@
         <v>30</v>
       </c>
       <c r="E10" s="4">
-        <v>0.69199999999999995</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="F10" s="6">
-        <v>5996.7</v>
+        <v>5052.1000000000004</v>
       </c>
       <c r="G10" s="6">
-        <v>11938.09</v>
+        <v>10077.99</v>
       </c>
       <c r="H10" s="6">
-        <v>24.177</v>
+        <v>24.584</v>
       </c>
       <c r="I10" s="6">
-        <v>5.9290000000000003</v>
+        <v>4.9509999999999996</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1097,16 +1096,16 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6">
-        <v>6.3520000000000003</v>
+        <v>5.7679999999999998</v>
       </c>
       <c r="Q10" s="6">
-        <v>8.5719999999999992</v>
+        <v>7.7279999999999998</v>
       </c>
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A11" s="5">
-        <v>44540</v>
+        <v>44561</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -1118,19 +1117,19 @@
         <v>31</v>
       </c>
       <c r="E11" s="4">
-        <v>0.70899999999999996</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="F11" s="6">
-        <v>5967</v>
+        <v>5041.6000000000004</v>
       </c>
       <c r="G11" s="6">
-        <v>11841.88</v>
+        <v>10019.280000000001</v>
       </c>
       <c r="H11" s="6">
-        <v>24.721</v>
+        <v>24.817</v>
       </c>
       <c r="I11" s="6">
-        <v>5.9240000000000004</v>
+        <v>4.5030000000000001</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1141,7 +1140,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6">
-        <v>25.802</v>
+        <v>25.076000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Updates to models, figures, etc.
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE80853-9D9A-48F0-9B8C-5E272ED80132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5195579-684B-4B33-906A-6830DDD67568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="18730" windowHeight="5860" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM Outputs" sheetId="1" r:id="rId1"/>
     <sheet name="Temp-Sal Values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -278,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +306,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +328,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -340,6 +364,25 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,8 +700,8 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -783,45 +826,51 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="A3" s="5">
+    <row r="3" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="7">
         <v>44539</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="9">
         <v>0.76200000000000001</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="10">
         <v>7453.3</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="10">
         <v>14805.92</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="10">
         <v>26.279</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="10">
         <v>2.2850000000000001</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A4" s="5">
@@ -1103,49 +1152,55 @@
       </c>
       <c r="R10" s="6"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="A11" s="5">
+    <row r="11" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A11" s="21">
         <v>44561</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="23">
         <v>0.61799999999999999</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="24">
         <v>5041.6000000000004</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="24">
         <v>10019.280000000001</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="24">
         <v>24.817</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="24">
         <v>4.5030000000000001</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6">
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24">
         <v>25.076000000000001</v>
       </c>
+      <c r="S11" s="22"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A12" s="5">
-        <v>44543</v>
+        <v>44567</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>34</v>
@@ -1166,7 +1221,7 @@
         <v>14493.3</v>
       </c>
       <c r="H12" s="6">
-        <v>27.952999999999999</v>
+        <v>27.652999999999999</v>
       </c>
       <c r="I12" s="6">
         <v>8.2319999999999993</v>
@@ -1183,7 +1238,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A13" s="5">
-        <v>44543</v>
+        <v>44567</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>34</v>
@@ -1195,7 +1250,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="4">
-        <v>0.70299999999999996</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="F13" s="6">
         <v>7216.7</v>
@@ -1221,49 +1276,55 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.75">
-      <c r="A14" s="5">
-        <v>44543</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A14" s="21">
+        <v>44567</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="9">
         <v>0.75</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="10">
         <v>7080.7</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="10">
         <v>14029.54</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10">
         <v>8.24</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K14" s="6">
-        <v>2.121</v>
-      </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="K14" s="10">
+        <v>2.12</v>
+      </c>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A15" s="5">
-        <v>44543</v>
+        <v>44567</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>34</v>
@@ -1301,49 +1362,55 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:24" s="15" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A16" s="5">
-        <v>44543</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>44567</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="13">
         <v>0.745</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="14">
         <v>7141.1</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="14">
         <v>14079</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="14">
         <v>27.234999999999999</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="14">
         <v>7.9779999999999998</v>
       </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6">
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14">
         <v>28.013000000000002</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A17" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -1355,19 +1422,19 @@
         <v>25</v>
       </c>
       <c r="E17" s="4">
-        <v>0.79200000000000004</v>
+        <v>0.79</v>
       </c>
       <c r="F17" s="6">
-        <v>3773.6</v>
+        <v>3622</v>
       </c>
       <c r="G17" s="6">
-        <v>7429.91</v>
+        <v>7129.7</v>
       </c>
       <c r="H17" s="6">
-        <v>28.07</v>
+        <v>28.067</v>
       </c>
       <c r="I17" s="6">
-        <v>5.67</v>
+        <v>5.665</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1379,9 +1446,9 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A18" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>34</v>
@@ -1393,19 +1460,19 @@
         <v>26</v>
       </c>
       <c r="E18" s="4">
-        <v>0.79400000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="F18" s="6">
-        <v>3768</v>
+        <v>3618.9</v>
       </c>
       <c r="G18" s="6">
-        <v>7414.87</v>
+        <v>7120.125</v>
       </c>
       <c r="H18" s="6">
-        <v>28.048999999999999</v>
+        <v>28.052</v>
       </c>
       <c r="I18" s="6">
-        <v>5.6559999999999997</v>
+        <v>5.6589999999999998</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1414,14 +1481,14 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6">
-        <v>3.59</v>
+        <v>3.706</v>
       </c>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A19" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>34</v>
@@ -1433,19 +1500,19 @@
         <v>29</v>
       </c>
       <c r="E19" s="4">
-        <v>0.81100000000000005</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="F19" s="6">
-        <v>3681.6</v>
+        <v>3533.9</v>
       </c>
       <c r="G19" s="6">
-        <v>7222.5429999999997</v>
+        <v>6933.48</v>
       </c>
       <c r="H19" s="6">
-        <v>28.073</v>
+        <v>28.030999999999999</v>
       </c>
       <c r="I19" s="6">
-        <v>5.38</v>
+        <v>5.3410000000000002</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1455,13 +1522,13 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6">
-        <v>8.4499999999999993</v>
+        <v>8.4190000000000005</v>
       </c>
       <c r="R19" s="6"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A20" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>34</v>
@@ -1473,19 +1540,19 @@
         <v>30</v>
       </c>
       <c r="E20" s="4">
-        <v>0.81299999999999994</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="F20" s="6">
-        <v>3672.6</v>
+        <v>3529.7</v>
       </c>
       <c r="G20" s="6">
-        <v>7199.55</v>
+        <v>6921.7</v>
       </c>
       <c r="H20" s="6">
-        <v>28.048999999999999</v>
+        <v>27.988</v>
       </c>
       <c r="I20" s="6">
-        <v>5.2859999999999996</v>
+        <v>5.258</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -1494,54 +1561,60 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6">
-        <v>4.1420000000000003</v>
+        <v>4.2539999999999996</v>
       </c>
       <c r="Q20" s="6">
-        <v>8.4740000000000002</v>
+        <v>8.4339999999999993</v>
       </c>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A21" s="5">
-        <v>44543</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>44574</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="4">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="F21" s="6">
-        <v>3600.6</v>
-      </c>
-      <c r="G21" s="6">
-        <v>7026.5</v>
-      </c>
-      <c r="H21" s="6">
-        <v>27.751000000000001</v>
-      </c>
-      <c r="I21" s="6">
-        <v>5.5129999999999999</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6">
-        <v>25.245999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="E21" s="9">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3464.8</v>
+      </c>
+      <c r="G21" s="10">
+        <v>6764.7809999999999</v>
+      </c>
+      <c r="H21" s="10">
+        <v>27.638000000000002</v>
+      </c>
+      <c r="I21" s="10">
+        <v>5.4859999999999998</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10">
+        <v>24.49</v>
+      </c>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A22" s="5">
         <v>44543</v>
       </c>
@@ -1579,7 +1652,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A23" s="5">
         <v>44543</v>
       </c>
@@ -1619,47 +1692,53 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.75">
-      <c r="A24" s="5">
+    <row r="24" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A24" s="21">
         <v>44543</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="23">
         <v>0.59199999999999997</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="24">
         <v>15110</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="24">
         <v>30202.71</v>
       </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6">
+      <c r="H24" s="24"/>
+      <c r="I24" s="24">
         <v>7.3559999999999999</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="6">
-        <v>1.0842000000000001</v>
-      </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="K24" s="24">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="22"/>
+      <c r="W24" s="22"/>
+      <c r="X24" s="22"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A25" s="5">
         <v>44543</v>
       </c>
@@ -1699,7 +1778,7 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A26" s="5">
         <v>44543</v>
       </c>
@@ -1739,7 +1818,7 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A27" s="5">
         <v>44543</v>
       </c>
@@ -1753,19 +1832,19 @@
         <v>25</v>
       </c>
       <c r="E27" s="4">
-        <v>0.65900000000000003</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F27" s="6">
-        <v>11069</v>
+        <v>10774</v>
       </c>
       <c r="G27" s="6">
-        <v>22167.02</v>
+        <v>21583.03</v>
       </c>
       <c r="H27" s="6">
-        <v>27.061</v>
+        <v>26.82</v>
       </c>
       <c r="I27" s="6">
-        <v>5.7320000000000002</v>
+        <v>5.6909999999999998</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -1777,7 +1856,7 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A28" s="5">
         <v>44543</v>
       </c>
@@ -1791,19 +1870,19 @@
         <v>26</v>
       </c>
       <c r="E28" s="4">
-        <v>0.67600000000000005</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="F28" s="6">
-        <v>11000</v>
+        <v>10706</v>
       </c>
       <c r="G28" s="6">
-        <v>22006.69</v>
+        <v>21419.37</v>
       </c>
       <c r="H28" s="6">
-        <v>26.87</v>
+        <v>26.620999999999999</v>
       </c>
       <c r="I28" s="6">
-        <v>5.758</v>
+        <v>5.726</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -1812,12 +1891,12 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6">
-        <v>7.99</v>
+        <v>8.3070000000000004</v>
       </c>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A29" s="5">
         <v>44543</v>
       </c>
@@ -1831,19 +1910,19 @@
         <v>29</v>
       </c>
       <c r="E29" s="4">
-        <v>0.70499999999999996</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="F29" s="6">
-        <v>10859</v>
+        <v>10580</v>
       </c>
       <c r="G29" s="6">
-        <v>21700.16</v>
+        <v>21150.03</v>
       </c>
       <c r="H29" s="6">
-        <v>27.701000000000001</v>
+        <v>27.599</v>
       </c>
       <c r="I29" s="6">
-        <v>5.6820000000000004</v>
+        <v>5.5940000000000003</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1853,11 +1932,11 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6">
-        <v>7.7389999999999999</v>
+        <v>7.6820000000000004</v>
       </c>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A30" s="5">
         <v>44543</v>
       </c>
@@ -1871,19 +1950,19 @@
         <v>30</v>
       </c>
       <c r="E30" s="4">
-        <v>0.71099999999999997</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="F30" s="6">
-        <v>10842</v>
+        <v>10563</v>
       </c>
       <c r="G30" s="6">
-        <v>21657.24</v>
+        <v>21100.87</v>
       </c>
       <c r="H30" s="6">
-        <v>27.603999999999999</v>
+        <v>27.491</v>
       </c>
       <c r="I30" s="6">
-        <v>5.6859999999999999</v>
+        <v>5.5949999999999998</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -1892,56 +1971,62 @@
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6">
-        <v>7.1870000000000003</v>
+        <v>7.56</v>
       </c>
       <c r="Q30" s="6">
-        <v>7.6719999999999997</v>
+        <v>7.5469999999999997</v>
       </c>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.75">
-      <c r="A31" s="5">
+    <row r="31" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A31" s="21">
         <v>44543</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="4">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="F31" s="6">
-        <v>10835</v>
-      </c>
-      <c r="G31" s="6">
-        <v>21635.51</v>
-      </c>
-      <c r="H31" s="6">
-        <v>27.58</v>
-      </c>
-      <c r="I31" s="6">
-        <v>5.6449999999999996</v>
-      </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6">
-        <v>23.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="E31" s="23">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="F31" s="24">
+        <v>10550</v>
+      </c>
+      <c r="G31" s="24">
+        <v>21063.29</v>
+      </c>
+      <c r="H31" s="24">
+        <v>27.481000000000002</v>
+      </c>
+      <c r="I31" s="24">
+        <v>5.5259999999999998</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24">
+        <v>23.94</v>
+      </c>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="22"/>
+      <c r="W31" s="22"/>
+      <c r="X31" s="22"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A32" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>41</v>
@@ -1953,19 +2038,19 @@
         <v>25</v>
       </c>
       <c r="E32" s="4">
-        <v>0.64900000000000002</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="F32" s="6">
-        <v>6128.5</v>
+        <v>6003.5</v>
       </c>
       <c r="G32" s="6">
-        <v>12221.21</v>
+        <v>11974.11</v>
       </c>
       <c r="H32" s="6">
-        <v>26.602</v>
+        <v>26.591000000000001</v>
       </c>
       <c r="I32" s="6">
-        <v>7.9160000000000004</v>
+        <v>7.9139999999999997</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -1977,9 +2062,9 @@
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A33" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>41</v>
@@ -1991,19 +2076,19 @@
         <v>26</v>
       </c>
       <c r="E33" s="4">
-        <v>0.65200000000000002</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F33" s="6">
-        <v>6125.9</v>
+        <v>6001</v>
       </c>
       <c r="G33" s="6">
-        <v>12211.7</v>
+        <v>11966.33</v>
       </c>
       <c r="H33" s="6">
-        <v>26.626999999999999</v>
+        <v>26.641999999999999</v>
       </c>
       <c r="I33" s="6">
-        <v>5.81</v>
+        <v>5.782</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -2012,14 +2097,14 @@
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6">
-        <v>5.0380000000000003</v>
+        <v>4.9489999999999998</v>
       </c>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A34" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>41</v>
@@ -2031,19 +2116,19 @@
         <v>29</v>
       </c>
       <c r="E34" s="4">
-        <v>0.68</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="F34" s="6">
-        <v>6031.7</v>
+        <v>5908.4</v>
       </c>
       <c r="G34" s="6">
-        <v>11994.29</v>
+        <v>11750.35</v>
       </c>
       <c r="H34" s="6">
-        <v>26.86</v>
+        <v>26.873999999999999</v>
       </c>
       <c r="I34" s="6">
-        <v>5.5780000000000003</v>
+        <v>5.5750000000000002</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -2053,13 +2138,13 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="6">
-        <v>8.6519999999999992</v>
+        <v>8.6419999999999995</v>
       </c>
       <c r="R34" s="6"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A35" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>41</v>
@@ -2071,19 +2156,19 @@
         <v>30</v>
       </c>
       <c r="E35" s="4">
-        <v>0.68100000000000005</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="F35" s="6">
-        <v>6033.1</v>
+        <v>5910.1</v>
       </c>
       <c r="G35" s="6">
-        <v>11998.75</v>
+        <v>11756.17</v>
       </c>
       <c r="H35" s="6">
-        <v>26.765000000000001</v>
+        <v>26.812000000000001</v>
       </c>
       <c r="I35" s="6">
-        <v>5.5519999999999996</v>
+        <v>5.5570000000000004</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -2092,56 +2177,62 @@
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6">
-        <v>2.9239999999999999</v>
+        <v>2.762</v>
       </c>
       <c r="Q35" s="6">
-        <v>8.657</v>
+        <v>8.6440000000000001</v>
       </c>
       <c r="R35" s="6"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A36" s="5">
-        <v>44543</v>
-      </c>
-      <c r="B36" s="1" t="s">
+        <v>44574</v>
+      </c>
+      <c r="B36" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="4">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="F36" s="6">
-        <v>5944.3</v>
-      </c>
-      <c r="G36" s="6">
-        <v>11791.08</v>
-      </c>
-      <c r="H36" s="6">
-        <v>26.198</v>
-      </c>
-      <c r="I36" s="6">
-        <v>5.55</v>
-      </c>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6">
-        <v>24.907</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="E36" s="23">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="F36" s="24">
+        <v>5869</v>
+      </c>
+      <c r="G36" s="24">
+        <v>11643.19</v>
+      </c>
+      <c r="H36" s="24">
+        <v>26.151</v>
+      </c>
+      <c r="I36" s="24">
+        <v>5.532</v>
+      </c>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24">
+        <v>24.853000000000002</v>
+      </c>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="22"/>
+      <c r="X36" s="22"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A37" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>42</v>
@@ -2153,19 +2244,19 @@
         <v>25</v>
       </c>
       <c r="E37" s="4">
-        <v>0.69399999999999995</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="F37" s="6">
-        <v>3839</v>
+        <v>3735.3</v>
       </c>
       <c r="G37" s="6">
-        <v>7603.26</v>
+        <v>7400.1</v>
       </c>
       <c r="H37" s="6">
-        <v>26.965</v>
+        <v>26.436</v>
       </c>
       <c r="I37" s="6">
-        <v>5.8869999999999996</v>
+        <v>7.0119999999999996</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -2177,9 +2268,9 @@
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A38" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
@@ -2191,19 +2282,19 @@
         <v>26</v>
       </c>
       <c r="E38" s="4">
-        <v>0.69899999999999995</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="F38" s="6">
-        <v>3826.2</v>
+        <v>3721.1</v>
       </c>
       <c r="G38" s="6">
-        <v>7574.18</v>
+        <v>7366.5</v>
       </c>
       <c r="H38" s="6">
-        <v>26.824999999999999</v>
+        <v>26.332000000000001</v>
       </c>
       <c r="I38" s="6">
-        <v>5.0330000000000004</v>
+        <v>5.4909999999999997</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -2212,14 +2303,14 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6">
-        <v>5.6509999999999998</v>
+        <v>6.2709999999999999</v>
       </c>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A39" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>42</v>
@@ -2231,19 +2322,19 @@
         <v>29</v>
       </c>
       <c r="E39" s="4">
-        <v>0.70199999999999996</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="F39" s="6">
-        <v>3819.7</v>
+        <v>3719.9</v>
       </c>
       <c r="G39" s="6">
-        <v>7553.2889999999998</v>
+        <v>7364.1</v>
       </c>
       <c r="H39" s="6">
-        <v>27.007000000000001</v>
+        <v>26.504999999999999</v>
       </c>
       <c r="I39" s="6">
-        <v>5.343</v>
+        <v>5.5309999999999997</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -2253,13 +2344,13 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="6">
-        <v>6.5869999999999997</v>
+        <v>5.6059999999999999</v>
       </c>
       <c r="R39" s="6"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A40" s="5">
-        <v>44543</v>
+        <v>44574</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>42</v>
@@ -2271,19 +2362,19 @@
         <v>30</v>
       </c>
       <c r="E40" s="4">
-        <v>0.70799999999999996</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="F40" s="6">
-        <v>3801.9</v>
+        <v>3697.2</v>
       </c>
       <c r="G40" s="6">
-        <v>7516.3310000000001</v>
+        <v>7315.8</v>
       </c>
       <c r="H40" s="6">
-        <v>26.861000000000001</v>
+        <v>26.369</v>
       </c>
       <c r="I40" s="6">
-        <v>5.0839999999999996</v>
+        <v>5.4020000000000001</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -2292,54 +2383,60 @@
       <c r="N40" s="6"/>
       <c r="O40" s="6"/>
       <c r="P40" s="6">
-        <v>5.73</v>
+        <v>5.7359999999999998</v>
       </c>
       <c r="Q40" s="6">
-        <v>6.008</v>
+        <v>4.5019999999999998</v>
       </c>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A41" s="5">
-        <v>44543</v>
-      </c>
-      <c r="B41" s="1" t="s">
+        <v>44574</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="4">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="F41" s="6">
-        <v>3754.3</v>
-      </c>
-      <c r="G41" s="6">
-        <v>7373.4189999999999</v>
-      </c>
-      <c r="H41" s="6">
-        <v>26.971</v>
-      </c>
-      <c r="I41" s="6">
-        <v>5.085</v>
-      </c>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6">
-        <v>24.41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="E41" s="23">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="F41" s="24">
+        <v>3649.4</v>
+      </c>
+      <c r="G41" s="24">
+        <v>7171.75</v>
+      </c>
+      <c r="H41" s="24">
+        <v>26.358000000000001</v>
+      </c>
+      <c r="I41" s="24">
+        <v>5.242</v>
+      </c>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24">
+        <v>24.132999999999999</v>
+      </c>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22"/>
+      <c r="X41" s="22"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A42" s="5">
         <v>44543</v>
       </c>
@@ -2377,7 +2474,7 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A43" s="5">
         <v>44543</v>
       </c>
@@ -2417,47 +2514,53 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.75">
-      <c r="A44" s="5">
+    <row r="44" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A44" s="16">
         <v>44543</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="18">
         <v>0.63200000000000001</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="19">
         <v>4580.7</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="19">
         <v>9004.2510000000002</v>
       </c>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19">
         <v>7.8869999999999996</v>
       </c>
-      <c r="J44" s="6" t="s">
+      <c r="J44" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K44" s="6">
+      <c r="K44" s="19">
         <v>2.2850000000000001</v>
       </c>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
+      <c r="X44" s="17"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A45" s="5">
         <v>44543</v>
       </c>
@@ -2497,7 +2600,7 @@
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A46" s="5">
         <v>44543</v>
       </c>
@@ -2537,7 +2640,7 @@
       <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A47" s="5">
         <v>44543</v>
       </c>
@@ -2575,7 +2678,7 @@
       <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A48" s="5">
         <v>44543</v>
       </c>
@@ -2615,7 +2718,7 @@
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A49" s="5">
         <v>44543</v>
       </c>
@@ -2655,7 +2758,7 @@
       </c>
       <c r="R49" s="6"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A50" s="5">
         <v>44543</v>
       </c>
@@ -2697,47 +2800,53 @@
       </c>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.75">
-      <c r="A51" s="5">
+    <row r="51" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A51" s="21">
         <v>44543</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="23">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="24">
         <v>3751.9</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="24">
         <v>7358.0079999999998</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H51" s="24">
         <v>25.966000000000001</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I51" s="24">
         <v>5.0709999999999997</v>
       </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6">
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24">
         <v>25.713000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.75">
+      <c r="S51" s="22"/>
+      <c r="T51" s="22"/>
+      <c r="U51" s="22"/>
+      <c r="V51" s="22"/>
+      <c r="W51" s="22"/>
+      <c r="X51" s="22"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E52" s="4"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
@@ -2753,7 +2862,7 @@
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E53" s="4"/>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
@@ -2769,7 +2878,7 @@
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E54" s="4"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
@@ -2785,7 +2894,7 @@
       <c r="Q54" s="6"/>
       <c r="R54" s="6"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E55" s="4"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
@@ -2801,7 +2910,7 @@
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E56" s="4"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
@@ -2817,7 +2926,7 @@
       <c r="Q56" s="6"/>
       <c r="R56" s="6"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E57" s="4"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
@@ -2833,7 +2942,7 @@
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E58" s="4"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
@@ -2849,7 +2958,7 @@
       <c r="Q58" s="6"/>
       <c r="R58" s="6"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E59" s="4"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
@@ -2865,7 +2974,7 @@
       <c r="Q59" s="6"/>
       <c r="R59" s="6"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E60" s="4"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
@@ -2881,7 +2990,7 @@
       <c r="Q60" s="6"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E61" s="4"/>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
@@ -2897,7 +3006,7 @@
       <c r="Q61" s="6"/>
       <c r="R61" s="6"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E62" s="4"/>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
@@ -2913,7 +3022,7 @@
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E63" s="4"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
@@ -2929,7 +3038,7 @@
       <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.75">
       <c r="E64" s="4"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>

</xml_diff>

<commit_message>
Updated code and figures
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5195579-684B-4B33-906A-6830DDD67568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13620754-FBF7-4AD7-A8C8-4D401F085F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="18730" windowHeight="5860" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM Outputs" sheetId="1" r:id="rId1"/>
@@ -700,8 +700,8 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
Organization and creation of streamlined RMD documents for each species.
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13620754-FBF7-4AD7-A8C8-4D401F085F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A6BA8F-B4C5-4DE7-8FB1-53D303D7A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Temp-Sal Values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="60">
   <si>
     <t>Species</t>
   </si>
@@ -273,6 +272,9 @@
   </si>
   <si>
     <t>Temp 3rd Quartile</t>
+  </si>
+  <si>
+    <t>enter</t>
   </si>
 </sst>
 </file>
@@ -699,9 +701,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0069B89D-77AC-4F26-B032-0EC1CFE3B568}">
   <dimension ref="A1:X114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1410,7 +1412,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A17" s="5">
-        <v>44574</v>
+        <v>44218</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>34</v>
@@ -1422,19 +1424,19 @@
         <v>25</v>
       </c>
       <c r="E17" s="4">
-        <v>0.79</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="F17" s="6">
-        <v>3622</v>
-      </c>
-      <c r="G17" s="6">
-        <v>7129.7</v>
+        <v>2731.6</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="H17" s="6">
-        <v>28.067</v>
+        <v>27.76</v>
       </c>
       <c r="I17" s="6">
-        <v>5.665</v>
+        <v>3.323</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1448,7 +1450,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A18" s="5">
-        <v>44574</v>
+        <v>44218</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>34</v>
@@ -1460,19 +1462,19 @@
         <v>26</v>
       </c>
       <c r="E18" s="4">
-        <v>0.79200000000000004</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="F18" s="6">
-        <v>3618.9</v>
-      </c>
-      <c r="G18" s="6">
-        <v>7120.125</v>
+        <v>2732.9</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="H18" s="6">
-        <v>28.052</v>
+        <v>27.760999999999999</v>
       </c>
       <c r="I18" s="6">
-        <v>5.6589999999999998</v>
+        <v>3.2229999999999999</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1481,14 +1483,14 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6">
-        <v>3.706</v>
+        <v>3.1589999999999998</v>
       </c>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A19" s="5">
-        <v>44574</v>
+        <v>44218</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>34</v>
@@ -1500,19 +1502,19 @@
         <v>29</v>
       </c>
       <c r="E19" s="4">
-        <v>0.80900000000000005</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="F19" s="6">
-        <v>3533.9</v>
-      </c>
-      <c r="G19" s="6">
-        <v>6933.48</v>
+        <v>2673.4</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="H19" s="6">
-        <v>28.030999999999999</v>
+        <v>27.472000000000001</v>
       </c>
       <c r="I19" s="6">
-        <v>5.3410000000000002</v>
+        <v>1.4710000000000001</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1522,13 +1524,13 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6">
-        <v>8.4190000000000005</v>
+        <v>6.6879999999999997</v>
       </c>
       <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.75">
       <c r="A20" s="5">
-        <v>44574</v>
+        <v>44218</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>34</v>
@@ -1540,19 +1542,19 @@
         <v>30</v>
       </c>
       <c r="E20" s="4">
-        <v>0.81100000000000005</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="F20" s="6">
-        <v>3529.7</v>
-      </c>
-      <c r="G20" s="6">
-        <v>6921.7</v>
+        <v>2668.3</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="H20" s="6">
-        <v>27.988</v>
+        <v>27.318999999999999</v>
       </c>
       <c r="I20" s="6">
-        <v>5.258</v>
+        <v>1</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -1561,16 +1563,16 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6">
-        <v>4.2539999999999996</v>
+        <v>4.6040000000000001</v>
       </c>
       <c r="Q20" s="6">
-        <v>8.4339999999999993</v>
+        <v>6.8239999999999998</v>
       </c>
       <c r="R20" s="6"/>
     </row>
     <row r="21" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A21" s="5">
-        <v>44574</v>
+        <v>44218</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>34</v>
@@ -1582,19 +1584,19 @@
         <v>31</v>
       </c>
       <c r="E21" s="9">
-        <v>0.82599999999999996</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="F21" s="10">
-        <v>3464.8</v>
-      </c>
-      <c r="G21" s="10">
-        <v>6764.7809999999999</v>
+        <v>2621.1</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="H21" s="10">
-        <v>27.638000000000002</v>
+        <v>26.69</v>
       </c>
       <c r="I21" s="10">
-        <v>5.4859999999999998</v>
+        <v>1.615</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -1605,7 +1607,7 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10">
-        <v>24.49</v>
+        <v>23.212</v>
       </c>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>

</xml_diff>

<commit_message>
Edits, adjustments, finalizing code
</commit_message>
<xml_diff>
--- a/GAM Models/GAM_Outputs.xlsx
+++ b/GAM Models/GAM_Outputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varyl\Desktop\GitHub\BeringSeaFishes_GAM_Analyses\GAM Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A6BA8F-B4C5-4DE7-8FB1-53D303D7A2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F732F1C6-06A1-43F1-9BFC-4EB539076826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{13C1DD21-5F2B-48D8-BB5C-3B8EFC3DE626}"/>
   </bookViews>
@@ -702,7 +702,7 @@
   <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>

</xml_diff>